<commit_message>
Trying to add midwater fish to code
</commit_message>
<xml_diff>
--- a/CODE/Data/three depths_preference matrix.xlsx
+++ b/CODE/Data/three depths_preference matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdvd\Dropbox\Werk\Overig\Meeting FEISTY\Colleen preference matrix 3 stages\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpetrik/Dropbox/Princeton/FEISTY/CODE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300BB9AC-6C23-447C-9857-A375F4349FC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B71B07-D9B6-EE49-8EB4-2C80822D232A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="theta-100m" sheetId="1" r:id="rId1"/>
@@ -920,18 +920,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -981,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>5.7940000000000004E-13</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>5.7940000000000004E-13</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>5.7940000000000004E-13</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>6.4384999999999998E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1620,9 +1620,9 @@
         <v>5.7940000000000004E-13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1">
         <v>1.5731999999999999E-14</v>
@@ -1673,7 +1673,7 @@
         <v>6.4384999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>5.7940000000000004E-13</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -1856,17 +1856,17 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1.6547E-15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>2.8177999999999999E-13</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>1.6547E-15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>2.6587E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>2.8177999999999999E-13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>6.9515000000000002E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>5.6190999999999998E-13</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -2786,18 +2786,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>1.7965E-17</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>2.8085000000000001E-13</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>1.7965E-17</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>2.6080999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>2.8085000000000001E-13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>3.4757999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>13</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>2.8094999999999998E-13</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>14</v>
       </c>

</xml_diff>